<commit_message>
wk3 notes and files
</commit_message>
<xml_diff>
--- a/xlfiles/Chapter2.xlsx
+++ b/xlfiles/Chapter2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bavanzi/Dropbox/Mac (3)/Documents/GitHub/ACTL20004-ACTL90021-2024/xlfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EB3351-18E8-FA43-B518-7431005AA44D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B2F308-B88F-FD4D-9366-B79019636F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="760" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{664FB022-1BC7-BB4C-9AD7-74455482708D}"/>
+    <workbookView xWindow="4880" yWindow="760" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{664FB022-1BC7-BB4C-9AD7-74455482708D}"/>
   </bookViews>
   <sheets>
     <sheet name="B.1 Exposure" sheetId="1" r:id="rId1"/>
@@ -4055,7 +4055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEFBD052-653A-4648-936E-EB05816D6A1F}">
   <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -4983,8 +4983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C27273-CD99-D446-9435-99E00B9EB402}">
   <dimension ref="A1:S56"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6581,7 +6581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7F00B14-29DD-164E-8437-4BB4341D5FD8}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
@@ -7870,7 +7870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41F6E75D-DECD-1D4E-8D9A-0AA868C6A453}">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -12284,7 +12284,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB2196EB-77E9-A746-98C8-C38437843E4E}">
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView topLeftCell="E34" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
@@ -14668,7 +14668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DA28597-9A62-DF4F-B1AB-39607C543170}">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>